<commit_message>
- experiment results (clean) - modified aggregated data
</commit_message>
<xml_diff>
--- a/2026-ECMFA/requests/experiment_design.xlsx
+++ b/2026-ECMFA/requests/experiment_design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\articles\2026\ECMFA.2026\LLM-model-assist\articles\ECMFA.2026\eval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos\emf-kaizen-experiments\2026-ECMFA\requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22D8AC7-1968-446B-9C4F-56F88165EB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F90AC-6411-4450-AA80-CCF79A8594AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D460A12-3815-4B88-B41B-94F6EEF2E6C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2D460A12-3815-4B88-B41B-94F6EEF2E6C3}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
-  <si>
-    <t>Metamodels</t>
-  </si>
-  <si>
-    <t>models</t>
-  </si>
-  <si>
-    <t>Types of requests</t>
-  </si>
-  <si>
-    <t>Concrete requests</t>
-  </si>
-  <si>
-    <t>LLMs</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="142">
   <si>
     <t>Meta-models</t>
   </si>
@@ -1288,698 +1273,652 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB327CA-7EAB-47A1-97C8-A5C4C6E76559}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="12" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="5" max="12" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E1" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E3" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="45"/>
+      <c r="G3" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="45"/>
+      <c r="I3" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="48"/>
+    </row>
+    <row r="4" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="38"/>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="12">
+        <v>10</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="39"/>
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1">
-        <v>1</v>
+      <c r="C7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="13">
+        <v>55</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
+    <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="42"/>
+      <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="C9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="12">
+        <v>12</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="10" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="43"/>
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="13">
+        <v>29</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <f>B1*B2*B3*B4*B5</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="45"/>
-      <c r="I9" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="48"/>
-    </row>
-    <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>6</v>
-      </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D11" s="11">
         <v>2</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>111</v>
+      <c r="E11" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="38"/>
       <c r="B12" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="D12" s="12">
         <v>10</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>114</v>
+        <v>86</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="39"/>
       <c r="B13" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="D13" s="13">
+        <v>21</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="38"/>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="12">
+        <v>10</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>129</v>
-      </c>
     </row>
-    <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="8" t="s">
+    <row r="16" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="39"/>
+      <c r="B16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="13">
+        <v>22</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="11">
-        <v>2</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>38</v>
+      <c r="H16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="12">
-        <v>12</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43"/>
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="13">
-        <v>29</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="K16" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="L16" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D17" s="11">
         <v>2</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>90</v>
+      <c r="E17" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>62</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
       <c r="B18" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="D18" s="12">
         <v>10</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>92</v>
+        <v>63</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="39"/>
       <c r="B19" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D19" s="13">
-        <v>21</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>94</v>
+        <v>20</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="11">
-        <v>1</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L20" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="12">
-        <v>10</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="13">
-        <v>22</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="K22" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="L22" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="11">
-        <v>2</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="K23" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="12">
-        <v>10</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J24" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="L24" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
-      <c r="B25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="13">
-        <v>20</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="K25" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="L25" s="20" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="E7:L7"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>